<commit_message>
rails: add challenge seeding
</commit_message>
<xml_diff>
--- a/lib/seed/challenges.xlsx
+++ b/lib/seed/challenges.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/src/osumb/challenges/spec/fixtures/seed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/src/osumb/challenges/lib/seed/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,67 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
-  <si>
-    <t>Hastings.286</t>
-  </si>
-  <si>
-    <t>Krebsbach.938</t>
-  </si>
-  <si>
-    <t>Slee.951</t>
-  </si>
-  <si>
-    <t>Faddis.634</t>
-  </si>
-  <si>
-    <t>Heal.856</t>
-  </si>
-  <si>
-    <t>I13</t>
-  </si>
-  <si>
-    <t>X14</t>
-  </si>
-  <si>
-    <t>S14</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>F13</t>
-  </si>
-  <si>
-    <t>H13</t>
-  </si>
-  <si>
-    <t>J13</t>
-  </si>
-  <si>
-    <t>E14</t>
-  </si>
-  <si>
-    <t>A14</t>
-  </si>
-  <si>
-    <t>L14</t>
-  </si>
-  <si>
-    <t>Wynter.419</t>
-  </si>
-  <si>
-    <t>Nordahl.9</t>
-  </si>
-  <si>
-    <t>Hosein.882</t>
-  </si>
-  <si>
-    <t>Imel.715</t>
-  </si>
-  <si>
-    <t>Parry.560</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>I3</t>
   </si>
@@ -119,13 +59,40 @@
     <t>K3</t>
   </si>
   <si>
-    <t>Challenger Spot</t>
-  </si>
-  <si>
-    <t>Challenger Name Number</t>
-  </si>
-  <si>
     <t>Spot Id</t>
+  </si>
+  <si>
+    <t>hastings.286</t>
+  </si>
+  <si>
+    <t>krebsbach.938</t>
+  </si>
+  <si>
+    <t>slee.951</t>
+  </si>
+  <si>
+    <t>faddis.634</t>
+  </si>
+  <si>
+    <t>heal.856</t>
+  </si>
+  <si>
+    <t>wynter.419</t>
+  </si>
+  <si>
+    <t>nordahl.9</t>
+  </si>
+  <si>
+    <t>hosein.882</t>
+  </si>
+  <si>
+    <t>imel.715</t>
+  </si>
+  <si>
+    <t>parry.560</t>
+  </si>
+  <si>
+    <t>Challenger Id</t>
   </si>
 </sst>
 </file>
@@ -447,137 +414,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B11" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rails: add seed data for past performance and link to challenges
</commit_message>
<xml_diff>
--- a/lib/seed/challenges.xlsx
+++ b/lib/seed/challenges.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18640" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>I3</t>
   </si>
@@ -93,6 +93,90 @@
   </si>
   <si>
     <t>Challenger Id</t>
+  </si>
+  <si>
+    <t>Winner Id</t>
+  </si>
+  <si>
+    <t>Challenger Comments</t>
+  </si>
+  <si>
+    <t>Challengee Comments</t>
+  </si>
+  <si>
+    <t>hagar.119</t>
+  </si>
+  <si>
+    <t>tindell.641</t>
+  </si>
+  <si>
+    <t>dias.832</t>
+  </si>
+  <si>
+    <t>borjas.78</t>
+  </si>
+  <si>
+    <t>tyree.611</t>
+  </si>
+  <si>
+    <t>Good 8x5 Horn not coming to parallel on sloopy Flashes not all the way up Good shoulders Playing endurance Phasing in ramp slow step</t>
+  </si>
+  <si>
+    <t>Good 8x5 Sloopy bell a little out and down Flashes not all the way up Shoulders not parallel on slides Playing endurance Ramp 8x5 inconsistent</t>
+  </si>
+  <si>
+    <t>body control -sloopy "yeah" angle -flash speed -hats off horns down angle -slow step bounce</t>
+  </si>
+  <si>
+    <t>8 to 5 long during choruses</t>
+  </si>
+  <si>
+    <t>Lean back on ups Stomp stomp on ramp Look really strong</t>
+  </si>
+  <si>
+    <t>- 8-5 short - box ttr - hesitation on slow step</t>
+  </si>
+  <si>
+    <t>Toes a bit behind knees in sloopy Horn off face during flashes Horn dip b low parallel</t>
+  </si>
+  <si>
+    <t>Horn dip below parallel</t>
+  </si>
+  <si>
+    <t>Great 8 to 5 at beginning. Better tone at beginning. Playing quality was more consistent throughout.</t>
+  </si>
+  <si>
+    <t>Slightly spurt at bringing. Flashing early. Horn bouncy cadences.</t>
+  </si>
+  <si>
+    <t>Horn got a little bouncy during tryout drill. Phasing during cadences. Drifted forward during slow step. Tended short during ramp. Doesn't dip in Sloopy.</t>
+  </si>
+  <si>
+    <t>Slight misses in 8 to 5 in tryout drill. Generally long during ramp. Kicking out Sloopy. Leg lift during step kicks was too low.</t>
+  </si>
+  <si>
+    <t>Good 8/5 Messed up step kicks Hats off horn angle back Mp back on ramp</t>
+  </si>
+  <si>
+    <t>Low horn angle, long 8/5 Missed playing out of flashes Mp up on ramp inconsist 8/5</t>
+  </si>
+  <si>
+    <t>Poor upper body and horn control Long 8/5 Sloopy legs low Looking at ground. 12/5 long Rushing slow step legs low</t>
+  </si>
+  <si>
+    <t>Long 8/5 Fracking notes sloopy 12/5 inconsistent but hitting. Missed notes out of flashes Legs a bit slow but up.</t>
+  </si>
+  <si>
+    <t>Sloopy is a little jerky Get legs up higher MP up in ramp</t>
+  </si>
+  <si>
+    <t>Long 8-5 Horn wrong angle at end of sloopy Horn is down in playing position</t>
+  </si>
+  <si>
+    <t>Horn arc looks a lot better Flashes cutting corners</t>
+  </si>
+  <si>
+    <t>Good first step Sometimes long 8-5 Sloopy Horn arc is good, but triangular Flashes slower than his Adjusted step/slow turn errors Horn angle on hats</t>
   </si>
 </sst>
 </file>
@@ -108,10 +192,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="12"/>
       <color rgb="FF353535"/>
-      <name val="PT Sans"/>
-      <charset val="204"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,8 +218,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -414,102 +499,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="A1:E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>